<commit_message>
Implementación de filtro para Región I, implementación de módulo de visualización, creación y edición de empleados y contratistas.
</commit_message>
<xml_diff>
--- a/public/templates/reporte.xlsx
+++ b/public/templates/reporte.xlsx
@@ -597,7 +597,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -730,21 +730,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -981,21 +966,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1120,7 +1090,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1239,16 +1209,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1263,7 +1233,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1272,10 +1242,10 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1284,36 +1254,36 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="41" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="41" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="41" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1347,10 +1317,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="51" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="49" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1371,10 +1341,10 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1399,14 +1369,14 @@
     <xf numFmtId="0" fontId="38" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1421,13 +1391,13 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1436,50 +1406,44 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="48" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1503,63 +1467,13 @@
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1568,17 +1482,55 @@
     <xf numFmtId="0" fontId="56" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="40" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="40" fillId="5" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="56" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="56" fillId="5" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1918,7 +1870,7 @@
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="40" zoomScaleNormal="80" zoomScaleSheetLayoutView="40" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="W33" sqref="W33"/>
+      <selection pane="bottomLeft" activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26.25"/>
@@ -2054,7 +2006,7 @@
       <c r="Y2" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="Z2" s="136"/>
+      <c r="Z2" s="134"/>
     </row>
     <row r="3" spans="1:26" s="44" customFormat="1" ht="47.25" thickBot="1">
       <c r="A3" s="87"/>
@@ -2102,10 +2054,10 @@
         <f t="shared" ref="X3:X33" si="1">SUM(M3:W3)</f>
         <v>0</v>
       </c>
-      <c r="Y3" s="139">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="171"/>
+      <c r="Y3" s="137">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="166"/>
     </row>
     <row r="4" spans="1:26" s="1" customFormat="1" ht="47.25" thickBot="1">
       <c r="A4" s="95"/>
@@ -2156,7 +2108,7 @@
       <c r="Y4" s="100">
         <v>0</v>
       </c>
-      <c r="Z4" s="172"/>
+      <c r="Z4" s="151"/>
     </row>
     <row r="5" spans="1:26" s="1" customFormat="1" ht="47.25" thickBot="1">
       <c r="A5" s="95"/>
@@ -2309,7 +2261,7 @@
       <c r="Y7" s="101">
         <v>0</v>
       </c>
-      <c r="Z7" s="151"/>
+      <c r="Z7" s="146"/>
     </row>
     <row r="8" spans="1:26" s="103" customFormat="1" ht="47.25" thickBot="1">
       <c r="A8" s="95"/>
@@ -2360,7 +2312,7 @@
       <c r="Y8" s="101">
         <v>0</v>
       </c>
-      <c r="Z8" s="151"/>
+      <c r="Z8" s="146"/>
     </row>
     <row r="9" spans="1:26" s="91" customFormat="1" ht="47.25" thickBot="1">
       <c r="A9" s="95"/>
@@ -2411,7 +2363,7 @@
       <c r="Y9" s="100">
         <v>0</v>
       </c>
-      <c r="Z9" s="149"/>
+      <c r="Z9" s="146"/>
     </row>
     <row r="10" spans="1:26" s="3" customFormat="1" ht="47.25" thickBot="1">
       <c r="A10" s="95"/>
@@ -2461,58 +2413,58 @@
       <c r="Y10" s="100">
         <v>0</v>
       </c>
-      <c r="Z10" s="169"/>
-    </row>
-    <row r="11" spans="1:26" s="125" customFormat="1" ht="47.25" thickBot="1">
-      <c r="A11" s="145"/>
-      <c r="B11" s="141"/>
-      <c r="C11" s="142">
+      <c r="Z10" s="149"/>
+    </row>
+    <row r="11" spans="1:26" s="124" customFormat="1" ht="47.25" thickBot="1">
+      <c r="A11" s="143"/>
+      <c r="B11" s="139"/>
+      <c r="C11" s="140">
         <v>1</v>
       </c>
-      <c r="D11" s="142">
+      <c r="D11" s="140">
         <v>1</v>
       </c>
-      <c r="E11" s="142">
-        <v>0</v>
-      </c>
-      <c r="F11" s="142">
+      <c r="E11" s="140">
+        <v>0</v>
+      </c>
+      <c r="F11" s="140">
         <v>1</v>
       </c>
-      <c r="G11" s="142">
-        <v>0</v>
-      </c>
-      <c r="H11" s="143">
+      <c r="G11" s="140">
+        <v>0</v>
+      </c>
+      <c r="H11" s="141">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I11" s="143"/>
-      <c r="J11" s="143"/>
-      <c r="K11" s="143">
+      <c r="I11" s="141"/>
+      <c r="J11" s="141"/>
+      <c r="K11" s="141">
         <f>SUM(H11:I11)</f>
         <v>3</v>
       </c>
-      <c r="L11" s="144">
+      <c r="L11" s="142">
         <v>3</v>
       </c>
-      <c r="M11" s="144"/>
-      <c r="N11" s="144"/>
-      <c r="O11" s="144"/>
-      <c r="P11" s="144"/>
-      <c r="Q11" s="144"/>
-      <c r="R11" s="144"/>
-      <c r="S11" s="144"/>
-      <c r="T11" s="144"/>
-      <c r="U11" s="144"/>
-      <c r="V11" s="144"/>
-      <c r="W11" s="146"/>
+      <c r="M11" s="142"/>
+      <c r="N11" s="142"/>
+      <c r="O11" s="142"/>
+      <c r="P11" s="142"/>
+      <c r="Q11" s="142"/>
+      <c r="R11" s="142"/>
+      <c r="S11" s="142"/>
+      <c r="T11" s="142"/>
+      <c r="U11" s="142"/>
+      <c r="V11" s="142"/>
+      <c r="W11" s="144"/>
       <c r="X11" s="123">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y11" s="140">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="173"/>
+      <c r="Y11" s="138">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="167"/>
     </row>
     <row r="12" spans="1:26" s="102" customFormat="1" ht="47.25" thickBot="1">
       <c r="A12" s="95"/>
@@ -2562,7 +2514,7 @@
       <c r="Y12" s="101">
         <v>0</v>
       </c>
-      <c r="Z12" s="150"/>
+      <c r="Z12" s="149"/>
     </row>
     <row r="13" spans="1:26" s="91" customFormat="1" ht="47.25" thickBot="1">
       <c r="A13" s="95"/>
@@ -2617,7 +2569,7 @@
       <c r="Y13" s="101">
         <v>0</v>
       </c>
-      <c r="Z13" s="151"/>
+      <c r="Z13" s="146"/>
     </row>
     <row r="14" spans="1:26" s="1" customFormat="1" ht="47.25" thickBot="1">
       <c r="A14" s="113"/>
@@ -2668,7 +2620,7 @@
       <c r="Y14" s="118">
         <v>0</v>
       </c>
-      <c r="Z14" s="169"/>
+      <c r="Z14" s="149"/>
     </row>
     <row r="15" spans="1:26" s="3" customFormat="1" ht="47.25" thickBot="1">
       <c r="A15" s="119"/>
@@ -2723,7 +2675,7 @@
       <c r="Y15" s="122">
         <v>0</v>
       </c>
-      <c r="Z15" s="152"/>
+      <c r="Z15" s="147"/>
     </row>
     <row r="16" spans="1:26" s="1" customFormat="1" ht="47.25" thickBot="1">
       <c r="A16" s="95"/>
@@ -2778,7 +2730,7 @@
       <c r="Y16" s="100">
         <v>0</v>
       </c>
-      <c r="Z16" s="149"/>
+      <c r="Z16" s="146"/>
     </row>
     <row r="17" spans="1:27" s="3" customFormat="1" ht="47.25" thickBot="1">
       <c r="A17" s="95"/>
@@ -2829,58 +2781,58 @@
       <c r="Y17" s="100">
         <v>0</v>
       </c>
-      <c r="Z17" s="151"/>
-    </row>
-    <row r="18" spans="1:27" s="126" customFormat="1" ht="47.25" thickBot="1">
-      <c r="A18" s="145"/>
-      <c r="B18" s="141"/>
-      <c r="C18" s="142">
+      <c r="Z17" s="146"/>
+    </row>
+    <row r="18" spans="1:27" s="125" customFormat="1" ht="47.25" thickBot="1">
+      <c r="A18" s="143"/>
+      <c r="B18" s="139"/>
+      <c r="C18" s="140">
         <v>1</v>
       </c>
-      <c r="D18" s="142">
-        <v>0</v>
-      </c>
-      <c r="E18" s="142">
-        <v>0</v>
-      </c>
-      <c r="F18" s="142">
-        <v>0</v>
-      </c>
-      <c r="G18" s="142">
-        <v>0</v>
-      </c>
-      <c r="H18" s="143">
+      <c r="D18" s="140">
+        <v>0</v>
+      </c>
+      <c r="E18" s="140">
+        <v>0</v>
+      </c>
+      <c r="F18" s="140">
+        <v>0</v>
+      </c>
+      <c r="G18" s="140">
+        <v>0</v>
+      </c>
+      <c r="H18" s="141">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I18" s="143"/>
-      <c r="J18" s="143"/>
-      <c r="K18" s="143">
+      <c r="I18" s="141"/>
+      <c r="J18" s="141"/>
+      <c r="K18" s="141">
         <f>SUM(H18:I18)</f>
         <v>1</v>
       </c>
-      <c r="L18" s="144">
+      <c r="L18" s="142">
         <v>1</v>
       </c>
-      <c r="M18" s="144"/>
-      <c r="N18" s="144"/>
-      <c r="O18" s="144"/>
-      <c r="P18" s="144"/>
-      <c r="Q18" s="144"/>
-      <c r="R18" s="144"/>
-      <c r="S18" s="144"/>
-      <c r="T18" s="144"/>
-      <c r="U18" s="144"/>
-      <c r="V18" s="144"/>
-      <c r="W18" s="146"/>
+      <c r="M18" s="142"/>
+      <c r="N18" s="142"/>
+      <c r="O18" s="142"/>
+      <c r="P18" s="142"/>
+      <c r="Q18" s="142"/>
+      <c r="R18" s="142"/>
+      <c r="S18" s="142"/>
+      <c r="T18" s="142"/>
+      <c r="U18" s="142"/>
+      <c r="V18" s="142"/>
+      <c r="W18" s="144"/>
       <c r="X18" s="123">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y18" s="140">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="173"/>
+      <c r="Y18" s="138">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="167"/>
     </row>
     <row r="19" spans="1:27" s="104" customFormat="1" ht="47.25" thickBot="1">
       <c r="A19" s="95"/>
@@ -2901,7 +2853,7 @@
         <v>0</v>
       </c>
       <c r="H19" s="98">
-        <f t="shared" ref="H19:H32" si="4">SUM(C19:G19)</f>
+        <f t="shared" ref="H19:H24" si="4">SUM(C19:G19)</f>
         <v>20</v>
       </c>
       <c r="I19" s="98">
@@ -2935,7 +2887,7 @@
       <c r="Y19" s="100">
         <v>0</v>
       </c>
-      <c r="Z19" s="153"/>
+      <c r="Z19" s="147"/>
     </row>
     <row r="20" spans="1:27" s="91" customFormat="1" ht="47.25" thickBot="1">
       <c r="A20" s="95"/>
@@ -2990,8 +2942,8 @@
       <c r="Y20" s="100">
         <v>0</v>
       </c>
-      <c r="Z20" s="149"/>
-      <c r="AA20" s="138"/>
+      <c r="Z20" s="146"/>
+      <c r="AA20" s="136"/>
     </row>
     <row r="21" spans="1:27" s="91" customFormat="1" ht="47.25" thickBot="1">
       <c r="A21" s="95"/>
@@ -3046,8 +2998,8 @@
       <c r="Y21" s="100">
         <v>0</v>
       </c>
-      <c r="Z21" s="154"/>
-      <c r="AA21" s="147"/>
+      <c r="Z21" s="148"/>
+      <c r="AA21" s="145"/>
     </row>
     <row r="22" spans="1:27" s="1" customFormat="1" ht="47.25" thickBot="1">
       <c r="A22" s="95"/>
@@ -3102,8 +3054,8 @@
       <c r="Y22" s="101">
         <v>0</v>
       </c>
-      <c r="Z22" s="169"/>
-      <c r="AA22" s="137"/>
+      <c r="Z22" s="149"/>
+      <c r="AA22" s="135"/>
     </row>
     <row r="23" spans="1:27" s="1" customFormat="1" ht="47.25" thickBot="1">
       <c r="A23" s="95"/>
@@ -3157,9 +3109,9 @@
       <c r="Y23" s="101">
         <v>0</v>
       </c>
-      <c r="Z23" s="149"/>
-    </row>
-    <row r="24" spans="1:27" s="1" customFormat="1" ht="46.5">
+      <c r="Z23" s="146"/>
+    </row>
+    <row r="24" spans="1:27" s="1" customFormat="1" ht="47.25" thickBot="1">
       <c r="A24" s="95"/>
       <c r="B24" s="96"/>
       <c r="C24" s="97">
@@ -3212,9 +3164,9 @@
       <c r="Y24" s="101">
         <v>0</v>
       </c>
-      <c r="Z24" s="151"/>
-    </row>
-    <row r="25" spans="1:27" s="1" customFormat="1" ht="46.5">
+      <c r="Z24" s="146"/>
+    </row>
+    <row r="25" spans="1:27" s="1" customFormat="1" ht="47.25" thickBot="1">
       <c r="A25" s="95"/>
       <c r="B25" s="96"/>
       <c r="C25" s="97"/>
@@ -3238,11 +3190,14 @@
       <c r="U25" s="98"/>
       <c r="V25" s="99"/>
       <c r="W25" s="121"/>
-      <c r="X25" s="124"/>
+      <c r="X25" s="123">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="Y25" s="101"/>
-      <c r="Z25" s="169"/>
-    </row>
-    <row r="26" spans="1:27" s="1" customFormat="1" ht="46.5">
+      <c r="Z25" s="149"/>
+    </row>
+    <row r="26" spans="1:27" s="1" customFormat="1" ht="47.25" thickBot="1">
       <c r="A26" s="95"/>
       <c r="B26" s="96"/>
       <c r="C26" s="97"/>
@@ -3266,11 +3221,14 @@
       <c r="U26" s="98"/>
       <c r="V26" s="99"/>
       <c r="W26" s="121"/>
-      <c r="X26" s="124"/>
+      <c r="X26" s="123">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="Y26" s="101"/>
-      <c r="Z26" s="149"/>
-    </row>
-    <row r="27" spans="1:27" s="1" customFormat="1" ht="46.5">
+      <c r="Z26" s="146"/>
+    </row>
+    <row r="27" spans="1:27" s="1" customFormat="1" ht="47.25" thickBot="1">
       <c r="A27" s="95"/>
       <c r="B27" s="96"/>
       <c r="C27" s="97"/>
@@ -3294,11 +3252,14 @@
       <c r="U27" s="99"/>
       <c r="V27" s="99"/>
       <c r="W27" s="121"/>
-      <c r="X27" s="124"/>
+      <c r="X27" s="123">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="Y27" s="100"/>
-      <c r="Z27" s="151"/>
-    </row>
-    <row r="28" spans="1:27" s="111" customFormat="1" ht="46.5">
+      <c r="Z27" s="146"/>
+    </row>
+    <row r="28" spans="1:27" s="111" customFormat="1" ht="47.25" thickBot="1">
       <c r="A28" s="105"/>
       <c r="B28" s="106"/>
       <c r="C28" s="107"/>
@@ -3322,11 +3283,14 @@
       <c r="U28" s="99"/>
       <c r="V28" s="99"/>
       <c r="W28" s="121"/>
-      <c r="X28" s="124"/>
+      <c r="X28" s="123">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="Y28" s="110"/>
-      <c r="Z28" s="170"/>
-    </row>
-    <row r="29" spans="1:27" s="1" customFormat="1" ht="46.5">
+      <c r="Z28" s="150"/>
+    </row>
+    <row r="29" spans="1:27" s="1" customFormat="1" ht="47.25" thickBot="1">
       <c r="A29" s="95"/>
       <c r="B29" s="96"/>
       <c r="C29" s="97"/>
@@ -3350,11 +3314,14 @@
       <c r="U29" s="99"/>
       <c r="V29" s="99"/>
       <c r="W29" s="121"/>
-      <c r="X29" s="124"/>
+      <c r="X29" s="123">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="Y29" s="101"/>
-      <c r="Z29" s="154"/>
-    </row>
-    <row r="30" spans="1:27" s="1" customFormat="1" ht="46.5">
+      <c r="Z29" s="148"/>
+    </row>
+    <row r="30" spans="1:27" s="1" customFormat="1" ht="47.25" thickBot="1">
       <c r="A30" s="95"/>
       <c r="B30" s="96"/>
       <c r="C30" s="97"/>
@@ -3378,11 +3345,14 @@
       <c r="U30" s="99"/>
       <c r="V30" s="99"/>
       <c r="W30" s="121"/>
-      <c r="X30" s="124"/>
+      <c r="X30" s="123">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="Y30" s="100"/>
-      <c r="Z30" s="169"/>
-    </row>
-    <row r="31" spans="1:27" s="1" customFormat="1" ht="46.5">
+      <c r="Z30" s="149"/>
+    </row>
+    <row r="31" spans="1:27" s="1" customFormat="1" ht="47.25" thickBot="1">
       <c r="A31" s="95"/>
       <c r="B31" s="96"/>
       <c r="C31" s="97"/>
@@ -3406,48 +3376,54 @@
       <c r="U31" s="99"/>
       <c r="V31" s="99"/>
       <c r="W31" s="121"/>
-      <c r="X31" s="124"/>
+      <c r="X31" s="123">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="Y31" s="100"/>
-      <c r="Z31" s="151"/>
+      <c r="Z31" s="146"/>
     </row>
     <row r="32" spans="1:27" s="3" customFormat="1" ht="47.25" thickBot="1">
-      <c r="A32" s="127"/>
-      <c r="B32" s="128"/>
-      <c r="C32" s="129"/>
-      <c r="D32" s="129"/>
-      <c r="E32" s="129"/>
-      <c r="F32" s="129"/>
-      <c r="G32" s="129"/>
-      <c r="H32" s="130"/>
-      <c r="I32" s="131"/>
-      <c r="J32" s="131"/>
-      <c r="K32" s="131"/>
-      <c r="L32" s="132"/>
-      <c r="M32" s="132"/>
-      <c r="N32" s="132"/>
-      <c r="O32" s="132"/>
-      <c r="P32" s="132"/>
-      <c r="Q32" s="132"/>
-      <c r="R32" s="132"/>
-      <c r="S32" s="132"/>
-      <c r="T32" s="132"/>
+      <c r="A32" s="126"/>
+      <c r="B32" s="127"/>
+      <c r="C32" s="128"/>
+      <c r="D32" s="128"/>
+      <c r="E32" s="128"/>
+      <c r="F32" s="128"/>
+      <c r="G32" s="128"/>
+      <c r="H32" s="129"/>
+      <c r="I32" s="130"/>
+      <c r="J32" s="130"/>
+      <c r="K32" s="130"/>
+      <c r="L32" s="131"/>
+      <c r="M32" s="131"/>
+      <c r="N32" s="131"/>
+      <c r="O32" s="131"/>
+      <c r="P32" s="131"/>
+      <c r="Q32" s="131"/>
+      <c r="R32" s="131"/>
+      <c r="S32" s="131"/>
+      <c r="T32" s="131"/>
       <c r="U32" s="116"/>
-      <c r="V32" s="132"/>
-      <c r="W32" s="133"/>
-      <c r="X32" s="134"/>
-      <c r="Y32" s="135"/>
+      <c r="V32" s="131"/>
+      <c r="W32" s="132"/>
+      <c r="X32" s="123">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y32" s="133"/>
       <c r="Z32" s="168"/>
     </row>
     <row r="33" spans="1:26" s="18" customFormat="1" ht="47.25" thickBot="1">
-      <c r="A33" s="155" t="s">
+      <c r="A33" s="153" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="156"/>
-      <c r="C33" s="156"/>
-      <c r="D33" s="156"/>
-      <c r="E33" s="156"/>
-      <c r="F33" s="156"/>
-      <c r="G33" s="156"/>
+      <c r="B33" s="154"/>
+      <c r="C33" s="154"/>
+      <c r="D33" s="154"/>
+      <c r="E33" s="154"/>
+      <c r="F33" s="154"/>
+      <c r="G33" s="154"/>
       <c r="H33" s="54"/>
       <c r="I33" s="55">
         <f>SUM(I31:I32)</f>
@@ -3494,7 +3470,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="U33" s="174">
+      <c r="U33" s="152">
         <f>SUM(U3:U32)</f>
         <v>0</v>
       </c>
@@ -3588,11 +3564,11 @@
       <c r="T37" s="77"/>
       <c r="U37" s="78"/>
       <c r="V37" s="79"/>
-      <c r="W37" s="157">
+      <c r="W37" s="155">
         <f>SUM(M33)</f>
         <v>0</v>
       </c>
-      <c r="X37" s="158"/>
+      <c r="X37" s="156"/>
       <c r="Y37" s="42"/>
       <c r="Z37" s="61"/>
     </row>
@@ -3609,11 +3585,11 @@
       <c r="T38" s="72"/>
       <c r="U38" s="73"/>
       <c r="V38" s="74"/>
-      <c r="W38" s="162">
+      <c r="W38" s="160">
         <f>SUM(N33)</f>
         <v>0</v>
       </c>
-      <c r="X38" s="163"/>
+      <c r="X38" s="161"/>
       <c r="Y38" s="42"/>
       <c r="Z38" s="62"/>
     </row>
@@ -3630,11 +3606,11 @@
       <c r="T39" s="72"/>
       <c r="U39" s="73"/>
       <c r="V39" s="74"/>
-      <c r="W39" s="162">
+      <c r="W39" s="160">
         <f>SUM(O33)</f>
         <v>0</v>
       </c>
-      <c r="X39" s="163"/>
+      <c r="X39" s="161"/>
       <c r="Y39" s="42"/>
       <c r="Z39" s="63"/>
     </row>
@@ -3651,10 +3627,10 @@
       <c r="T40" s="72"/>
       <c r="U40" s="73"/>
       <c r="V40" s="74"/>
-      <c r="W40" s="162">
-        <v>0</v>
-      </c>
-      <c r="X40" s="163"/>
+      <c r="W40" s="160">
+        <v>0</v>
+      </c>
+      <c r="X40" s="161"/>
       <c r="Y40" s="42"/>
       <c r="Z40" s="64"/>
     </row>
@@ -3680,11 +3656,11 @@
       <c r="T41" s="72"/>
       <c r="U41" s="73"/>
       <c r="V41" s="74"/>
-      <c r="W41" s="162">
+      <c r="W41" s="160">
         <f>SUM(Q33)</f>
         <v>0</v>
       </c>
-      <c r="X41" s="163"/>
+      <c r="X41" s="161"/>
       <c r="Y41" s="42"/>
       <c r="Z41" s="14"/>
     </row>
@@ -3699,11 +3675,11 @@
       <c r="T42" s="72"/>
       <c r="U42" s="73"/>
       <c r="V42" s="74"/>
-      <c r="W42" s="162">
+      <c r="W42" s="160">
         <f>SUM(R33)</f>
         <v>0</v>
       </c>
-      <c r="X42" s="163"/>
+      <c r="X42" s="161"/>
       <c r="Y42" s="42"/>
       <c r="Z42" s="14"/>
     </row>
@@ -3718,11 +3694,11 @@
       <c r="T43" s="72"/>
       <c r="U43" s="73"/>
       <c r="V43" s="74"/>
-      <c r="W43" s="162">
+      <c r="W43" s="160">
         <f>SUM(S33)</f>
         <v>0</v>
       </c>
-      <c r="X43" s="163"/>
+      <c r="X43" s="161"/>
       <c r="Y43" s="42"/>
       <c r="Z43" s="42"/>
     </row>
@@ -3742,11 +3718,11 @@
       <c r="T44" s="72"/>
       <c r="U44" s="73"/>
       <c r="V44" s="74"/>
-      <c r="W44" s="162">
+      <c r="W44" s="160">
         <f>SUM(T33)</f>
         <v>0</v>
       </c>
-      <c r="X44" s="163"/>
+      <c r="X44" s="161"/>
       <c r="Y44" s="42"/>
       <c r="Z44" s="14"/>
     </row>
@@ -3766,11 +3742,11 @@
       <c r="T45" s="72"/>
       <c r="U45" s="73"/>
       <c r="V45" s="74"/>
-      <c r="W45" s="162">
+      <c r="W45" s="160">
         <f>SUM(U33)</f>
         <v>0</v>
       </c>
-      <c r="X45" s="163"/>
+      <c r="X45" s="161"/>
       <c r="Y45" s="42"/>
       <c r="Z45" s="14"/>
     </row>
@@ -3796,11 +3772,11 @@
       <c r="T46" s="72"/>
       <c r="U46" s="70"/>
       <c r="V46" s="71"/>
-      <c r="W46" s="166">
+      <c r="W46" s="164">
         <f>SUM(W33)</f>
         <v>0</v>
       </c>
-      <c r="X46" s="167"/>
+      <c r="X46" s="165"/>
       <c r="Y46" s="42"/>
       <c r="Z46" s="15"/>
     </row>
@@ -3818,21 +3794,21 @@
       <c r="L47" s="28"/>
       <c r="M47" s="31"/>
       <c r="N47" s="31"/>
-      <c r="O47" s="159" t="s">
+      <c r="O47" s="157" t="s">
         <v>29</v>
       </c>
-      <c r="P47" s="160"/>
-      <c r="Q47" s="160"/>
-      <c r="R47" s="160"/>
-      <c r="S47" s="160"/>
-      <c r="T47" s="160"/>
-      <c r="U47" s="161"/>
+      <c r="P47" s="158"/>
+      <c r="Q47" s="158"/>
+      <c r="R47" s="158"/>
+      <c r="S47" s="158"/>
+      <c r="T47" s="158"/>
+      <c r="U47" s="159"/>
       <c r="V47" s="75"/>
-      <c r="W47" s="164">
+      <c r="W47" s="162">
         <f>SUM(W37:X46)</f>
         <v>0</v>
       </c>
-      <c r="X47" s="165"/>
+      <c r="X47" s="163"/>
       <c r="Z47" s="15"/>
     </row>
     <row r="48" spans="1:26" s="12" customFormat="1" ht="30" customHeight="1">

</xml_diff>